<commit_message>
fix bug of prediction
</commit_message>
<xml_diff>
--- a/output/experiments/Aug2023_debug/debug.xlsx
+++ b/output/experiments/Aug2023_debug/debug.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="94">
   <si>
     <t>status</t>
   </si>
@@ -163,6 +163,12 @@
     <t>grid_max</t>
   </si>
   <si>
+    <t>bat_e_terminal</t>
+  </si>
+  <si>
+    <t>bat_e_terminal_revenue</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -193,6 +199,15 @@
     <t>GT</t>
   </si>
   <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
     <t>unconscious</t>
   </si>
   <si>
@@ -202,6 +217,9 @@
     <t>3-2-12-0</t>
   </si>
   <si>
+    <t>3-15-12-0</t>
+  </si>
+  <si>
     <t>moving</t>
   </si>
   <si>
@@ -227,6 +245,57 @@
   </si>
   <si>
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-440-unconscious-3-1-12-0-3-2-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-18_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-RBC-MSC-GT-unconscious-1.5-0.6-0.6-unif-439-unconscious-3-1-12-0-3-15-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-21_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-439-unconscious-3-1-12-0-3-15-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-21_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-RBC-MSC-GT-unconscious-1.5-0.6-0.6-unif-440-unconscious-3-1-12-0-3-15-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-21_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-440-unconscious-3-1-12-0-3-15-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-21_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-RBC-MSC-GT-unconscious-1.5-0.6-0.6-unif-441-unconscious-3-1-12-0-3-15-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-21_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-441-unconscious-3-1-12-0-3-15-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-21_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-RBC-MSC-GT-unconscious-1.5-0.6-0.6-unif-442-unconscious-3-1-12-0-3-15-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-21_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-442-unconscious-3-1-12-0-3-15-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-21_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-RBC-MSC-GT-unconscious-1.5-0.6-0.6-unif-443-unconscious-3-1-12-0-3-15-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-22_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-443-unconscious-3-1-12-0-3-2-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-22_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-RBC-MSC-Simple-unconscious-1.5-0.6-0.6-unif-444-unconscious-3-1-12-0-3-2-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-22_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Naive-unconscious-1.5-0.6-0.6-flex-444-unconscious-3-1-12-0-3-2-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-22_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Prediction-unconscious-1.5-0.6-0.6-flex-444-unconscious-3-1-12-0-3-2-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-22_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Prediction-unconscious-1.5-0.6-0.6-flex-445-unconscious-3-1-12-0-3-2-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-22_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Prediction-unconscious-1.5-0.6-0.6-flex-446-unconscious-3-1-12-0-3-2-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-22_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Prediction-unconscious-1.5-0.6-0.6-flex-447-unconscious-3-1-12-0-3-2-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-22_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Prediction-unconscious-1.5-0.6-0.6-flex-448-unconscious-3-1-12-0-3-2-12-0-Sum-GILMAN-Sum-moving-0-0-2023-08-22_001.xlsx</t>
   </si>
 </sst>
 </file>
@@ -584,15 +653,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX7"/>
+  <dimension ref="A1:AZ24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:50">
+    <row r="1" spans="1:52">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -741,46 +810,52 @@
       <c r="AX1" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="AY1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:52">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H2">
         <v>438</v>
       </c>
       <c r="I2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="L2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="N2">
         <v>27</v>
@@ -792,7 +867,7 @@
         <v>0.6</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -801,7 +876,7 @@
         <v>0.6</v>
       </c>
       <c r="T2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -816,7 +891,7 @@
         <v>10.5020567</v>
       </c>
       <c r="Y2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="Z2">
         <v>411.6439873490882</v>
@@ -888,45 +963,45 @@
         <v>145.4345719263315</v>
       </c>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:52">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H3">
         <v>438</v>
       </c>
       <c r="I3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="N3">
         <v>27</v>
@@ -938,7 +1013,7 @@
         <v>0.6</v>
       </c>
       <c r="Q3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -947,7 +1022,7 @@
         <v>0.6</v>
       </c>
       <c r="T3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -962,7 +1037,7 @@
         <v>28.9158686</v>
       </c>
       <c r="Y3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="Z3">
         <v>394.5323092879937</v>
@@ -1034,45 +1109,45 @@
         <v>180.9148635901386</v>
       </c>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:52">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H4">
         <v>439</v>
       </c>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="K4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="L4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="N4">
         <v>27</v>
@@ -1084,7 +1159,7 @@
         <v>0.6</v>
       </c>
       <c r="Q4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -1093,7 +1168,7 @@
         <v>0.6</v>
       </c>
       <c r="T4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -1108,7 +1183,7 @@
         <v>9.628790499999999</v>
       </c>
       <c r="Y4" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="Z4">
         <v>381.0232060827013</v>
@@ -1180,45 +1255,45 @@
         <v>120.5724742197953</v>
       </c>
     </row>
-    <row r="5" spans="1:50">
+    <row r="5" spans="1:52">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H5">
         <v>439</v>
       </c>
       <c r="I5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J5" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="N5">
         <v>27</v>
@@ -1230,7 +1305,7 @@
         <v>0.6</v>
       </c>
       <c r="Q5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -1239,7 +1314,7 @@
         <v>0.6</v>
       </c>
       <c r="T5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -1254,7 +1329,7 @@
         <v>25.0494701</v>
       </c>
       <c r="Y5" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="Z5">
         <v>345.2214350104221</v>
@@ -1326,45 +1401,45 @@
         <v>96.51104167448554</v>
       </c>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:52">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H6">
         <v>440</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="K6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="L6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M6" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="N6">
         <v>27</v>
@@ -1376,7 +1451,7 @@
         <v>0.6</v>
       </c>
       <c r="Q6" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1385,7 +1460,7 @@
         <v>0.6</v>
       </c>
       <c r="T6" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -1400,7 +1475,7 @@
         <v>10.0712798</v>
       </c>
       <c r="Y6" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="Z6">
         <v>397.5622426972881</v>
@@ -1472,45 +1547,45 @@
         <v>120.5724742197953</v>
       </c>
     </row>
-    <row r="7" spans="1:50">
+    <row r="7" spans="1:52">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H7">
         <v>440</v>
       </c>
       <c r="I7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="L7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M7" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="N7">
         <v>27</v>
@@ -1522,7 +1597,7 @@
         <v>0.6</v>
       </c>
       <c r="Q7" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -1531,7 +1606,7 @@
         <v>0.6</v>
       </c>
       <c r="T7" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -1546,7 +1621,7 @@
         <v>24.6537524</v>
       </c>
       <c r="Y7" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="Z7">
         <v>374.9810199737852</v>
@@ -1616,6 +1691,1582 @@
       </c>
       <c r="AX7">
         <v>102.399657524847</v>
+      </c>
+    </row>
+    <row r="8" spans="1:52">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8">
+        <v>439</v>
+      </c>
+      <c r="I8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8">
+        <v>27</v>
+      </c>
+      <c r="O8">
+        <v>1.5</v>
+      </c>
+      <c r="P8">
+        <v>0.6</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>68</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0.6</v>
+      </c>
+      <c r="T8" t="s">
+        <v>69</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9">
+        <v>439</v>
+      </c>
+      <c r="I9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M9" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9">
+        <v>27</v>
+      </c>
+      <c r="O9">
+        <v>1.5</v>
+      </c>
+      <c r="P9">
+        <v>0.6</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>68</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0.6</v>
+      </c>
+      <c r="T9" t="s">
+        <v>70</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:52">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10">
+        <v>440</v>
+      </c>
+      <c r="I10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" t="s">
+        <v>65</v>
+      </c>
+      <c r="M10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10">
+        <v>27</v>
+      </c>
+      <c r="O10">
+        <v>1.5</v>
+      </c>
+      <c r="P10">
+        <v>0.6</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>68</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0.6</v>
+      </c>
+      <c r="T10" t="s">
+        <v>69</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:52">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11">
+        <v>440</v>
+      </c>
+      <c r="I11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M11" t="s">
+        <v>67</v>
+      </c>
+      <c r="N11">
+        <v>27</v>
+      </c>
+      <c r="O11">
+        <v>1.5</v>
+      </c>
+      <c r="P11">
+        <v>0.6</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>68</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0.6</v>
+      </c>
+      <c r="T11" t="s">
+        <v>70</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12">
+        <v>441</v>
+      </c>
+      <c r="I12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" t="s">
+        <v>65</v>
+      </c>
+      <c r="M12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N12">
+        <v>27</v>
+      </c>
+      <c r="O12">
+        <v>1.5</v>
+      </c>
+      <c r="P12">
+        <v>0.6</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>68</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0.6</v>
+      </c>
+      <c r="T12" t="s">
+        <v>69</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:52">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13">
+        <v>441</v>
+      </c>
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" t="s">
+        <v>65</v>
+      </c>
+      <c r="M13" t="s">
+        <v>67</v>
+      </c>
+      <c r="N13">
+        <v>27</v>
+      </c>
+      <c r="O13">
+        <v>1.5</v>
+      </c>
+      <c r="P13">
+        <v>0.6</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>68</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0.6</v>
+      </c>
+      <c r="T13" t="s">
+        <v>70</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:52">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14">
+        <v>442</v>
+      </c>
+      <c r="I14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" t="s">
+        <v>65</v>
+      </c>
+      <c r="M14" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14">
+        <v>27</v>
+      </c>
+      <c r="O14">
+        <v>1.5</v>
+      </c>
+      <c r="P14">
+        <v>0.6</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>68</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0.6</v>
+      </c>
+      <c r="T14" t="s">
+        <v>69</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15">
+        <v>442</v>
+      </c>
+      <c r="I15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15" t="s">
+        <v>65</v>
+      </c>
+      <c r="M15" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15">
+        <v>27</v>
+      </c>
+      <c r="O15">
+        <v>1.5</v>
+      </c>
+      <c r="P15">
+        <v>0.6</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>68</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0.6</v>
+      </c>
+      <c r="T15" t="s">
+        <v>70</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:52">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16">
+        <v>443</v>
+      </c>
+      <c r="I16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16" t="s">
+        <v>65</v>
+      </c>
+      <c r="M16" t="s">
+        <v>67</v>
+      </c>
+      <c r="N16">
+        <v>27</v>
+      </c>
+      <c r="O16">
+        <v>1.5</v>
+      </c>
+      <c r="P16">
+        <v>0.6</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>68</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0.6</v>
+      </c>
+      <c r="T16" t="s">
+        <v>69</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>420.2934703871548</v>
+      </c>
+      <c r="W16">
+        <v>13.98958333333333</v>
+      </c>
+      <c r="X16">
+        <v>199.6670412</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z16">
+        <v>420.2934703871548</v>
+      </c>
+      <c r="AA16">
+        <v>402.0879909351</v>
+      </c>
+      <c r="AB16">
+        <v>18.2054794520548</v>
+      </c>
+      <c r="AC16">
+        <v>18.2054794520548</v>
+      </c>
+      <c r="AD16">
+        <v>443</v>
+      </c>
+      <c r="AE16">
+        <v>5.485361946138177</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <v>0.1737713480666503</v>
+      </c>
+      <c r="AI16">
+        <v>0.1737713480666503</v>
+      </c>
+      <c r="AJ16">
+        <v>0.166244248719451</v>
+      </c>
+      <c r="AL16">
+        <v>101.1282766426143</v>
+      </c>
+      <c r="AM16">
+        <v>300.9597142924857</v>
+      </c>
+      <c r="AO16">
+        <v>53.18242740134028</v>
+      </c>
+      <c r="AP16">
+        <v>1938.249490990321</v>
+      </c>
+      <c r="AQ16">
+        <v>480.4085620389424</v>
+      </c>
+      <c r="AR16">
+        <v>2418.658053029264</v>
+      </c>
+      <c r="AS16">
+        <v>772.0069153932595</v>
+      </c>
+      <c r="AT16">
+        <v>1649.697142713826</v>
+      </c>
+      <c r="AU16">
+        <v>1.396990691459563</v>
+      </c>
+      <c r="AV16">
+        <v>301.0713486020147</v>
+      </c>
+      <c r="AW16">
+        <v>0.1116343095290732</v>
+      </c>
+      <c r="AX16">
+        <v>168.5471277376905</v>
+      </c>
+      <c r="AY16">
+        <v>0</v>
+      </c>
+      <c r="AZ16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:52">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17">
+        <v>443</v>
+      </c>
+      <c r="I17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K17" t="s">
+        <v>64</v>
+      </c>
+      <c r="L17" t="s">
+        <v>65</v>
+      </c>
+      <c r="M17" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17">
+        <v>27</v>
+      </c>
+      <c r="O17">
+        <v>1.5</v>
+      </c>
+      <c r="P17">
+        <v>0.6</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>68</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0.6</v>
+      </c>
+      <c r="T17" t="s">
+        <v>70</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>326.4411462373438</v>
+      </c>
+      <c r="W17">
+        <v>0.9895833333333334</v>
+      </c>
+      <c r="X17">
+        <v>393.1796861</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z17">
+        <v>326.4411462373438</v>
+      </c>
+      <c r="AA17">
+        <v>308.235666785289</v>
+      </c>
+      <c r="AB17">
+        <v>18.2054794520548</v>
+      </c>
+      <c r="AC17">
+        <v>18.2054794520548</v>
+      </c>
+      <c r="AD17">
+        <v>443</v>
+      </c>
+      <c r="AE17">
+        <v>5.744679994296956</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <v>0</v>
+      </c>
+      <c r="AH17">
+        <v>0.1576124597042513</v>
+      </c>
+      <c r="AI17">
+        <v>0.1576124597042513</v>
+      </c>
+      <c r="AJ17">
+        <v>0.1488224820019695</v>
+      </c>
+      <c r="AL17">
+        <v>61.43979451490778</v>
+      </c>
+      <c r="AM17">
+        <v>295.6577673566699</v>
+      </c>
+      <c r="AO17">
+        <v>34.35789473684211</v>
+      </c>
+      <c r="AP17">
+        <v>1850.755831578946</v>
+      </c>
+      <c r="AQ17">
+        <v>220.4074942766856</v>
+      </c>
+      <c r="AR17">
+        <v>2071.163325855632</v>
+      </c>
+      <c r="AS17">
+        <v>446.2578682383618</v>
+      </c>
+      <c r="AT17">
+        <v>1909.702321994374</v>
+      </c>
+      <c r="AU17">
+        <v>0.7293662728249202</v>
+      </c>
+      <c r="AV17">
+        <v>295.7798632707407</v>
+      </c>
+      <c r="AW17">
+        <v>0.1220959140708917</v>
+      </c>
+      <c r="AX17">
+        <v>102.3996575248463</v>
+      </c>
+      <c r="AY17">
+        <v>287.1384407520361</v>
+      </c>
+      <c r="AZ17">
+        <v>48.86189508628859</v>
+      </c>
+    </row>
+    <row r="18" spans="1:52">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18">
+        <v>444</v>
+      </c>
+      <c r="I18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" t="s">
+        <v>64</v>
+      </c>
+      <c r="K18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L18" t="s">
+        <v>65</v>
+      </c>
+      <c r="M18" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18">
+        <v>27</v>
+      </c>
+      <c r="O18">
+        <v>1.5</v>
+      </c>
+      <c r="P18">
+        <v>0.6</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>68</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0.6</v>
+      </c>
+      <c r="T18" t="s">
+        <v>69</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>397.9243952510444</v>
+      </c>
+      <c r="W18">
+        <v>0.9895833333333334</v>
+      </c>
+      <c r="X18">
+        <v>82.9151821</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z18">
+        <v>397.9243952510444</v>
+      </c>
+      <c r="AA18">
+        <v>379.6778199085786</v>
+      </c>
+      <c r="AB18">
+        <v>18.24657534246575</v>
+      </c>
+      <c r="AC18">
+        <v>18.24657534246575</v>
+      </c>
+      <c r="AD18">
+        <v>444</v>
+      </c>
+      <c r="AE18">
+        <v>5.75764766922765</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <v>0.1917551251176552</v>
+      </c>
+      <c r="AI18">
+        <v>0.1917551251176552</v>
+      </c>
+      <c r="AJ18">
+        <v>0.1829623132681684</v>
+      </c>
+      <c r="AL18">
+        <v>73.20865134486243</v>
+      </c>
+      <c r="AM18">
+        <v>306.4691685637162</v>
+      </c>
+      <c r="AO18">
+        <v>34.35789473684211</v>
+      </c>
+      <c r="AP18">
+        <v>1850.755831578946</v>
+      </c>
+      <c r="AQ18">
+        <v>224.4137108616531</v>
+      </c>
+      <c r="AR18">
+        <v>2075.169542440599</v>
+      </c>
+      <c r="AS18">
+        <v>446.2578682383618</v>
+      </c>
+      <c r="AT18">
+        <v>1625.666143248221</v>
+      </c>
+      <c r="AU18">
+        <v>0</v>
+      </c>
+      <c r="AV18">
+        <v>306.4691685637162</v>
+      </c>
+      <c r="AW18">
+        <v>0</v>
+      </c>
+      <c r="AX18">
+        <v>122.014418908104</v>
+      </c>
+      <c r="AY18">
+        <v>0</v>
+      </c>
+      <c r="AZ18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:52">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19">
+        <v>444</v>
+      </c>
+      <c r="I19" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19" t="s">
+        <v>64</v>
+      </c>
+      <c r="L19" t="s">
+        <v>65</v>
+      </c>
+      <c r="M19" t="s">
+        <v>66</v>
+      </c>
+      <c r="N19">
+        <v>27</v>
+      </c>
+      <c r="O19">
+        <v>1.5</v>
+      </c>
+      <c r="P19">
+        <v>0.6</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>68</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0.6</v>
+      </c>
+      <c r="T19" t="s">
+        <v>70</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>337.4694552698268</v>
+      </c>
+      <c r="W19">
+        <v>0.9895833333333334</v>
+      </c>
+      <c r="X19">
+        <v>17.0448289</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z19">
+        <v>337.4694552698268</v>
+      </c>
+      <c r="AA19">
+        <v>319.2228799273611</v>
+      </c>
+      <c r="AB19">
+        <v>18.24657534246575</v>
+      </c>
+      <c r="AC19">
+        <v>18.24657534246575</v>
+      </c>
+      <c r="AD19">
+        <v>444</v>
+      </c>
+      <c r="AE19">
+        <v>5.75764766922765</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AH19">
+        <v>0.1612386576476962</v>
+      </c>
+      <c r="AI19">
+        <v>0.1612386576476962</v>
+      </c>
+      <c r="AJ19">
+        <v>0.1525206736377526</v>
+      </c>
+      <c r="AL19">
+        <v>91.98710279675198</v>
+      </c>
+      <c r="AM19">
+        <v>270.0320825760696</v>
+      </c>
+      <c r="AO19">
+        <v>34.35789473684211</v>
+      </c>
+      <c r="AP19">
+        <v>1850.755831578946</v>
+      </c>
+      <c r="AQ19">
+        <v>242.2252201933405</v>
+      </c>
+      <c r="AR19">
+        <v>2092.981051772287</v>
+      </c>
+      <c r="AS19">
+        <v>446.2578682383618</v>
+      </c>
+      <c r="AT19">
+        <v>1901.784729127828</v>
+      </c>
+      <c r="AU19">
+        <v>7.809248378088083</v>
+      </c>
+      <c r="AV19">
+        <v>271.2730729659299</v>
+      </c>
+      <c r="AW19">
+        <v>1.240990389860366</v>
+      </c>
+      <c r="AX19">
+        <v>153.3118379945867</v>
+      </c>
+      <c r="AY19">
+        <v>251.493815249211</v>
+      </c>
+      <c r="AZ19">
+        <v>42.79630544546048</v>
+      </c>
+    </row>
+    <row r="20" spans="1:52">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20">
+        <v>444</v>
+      </c>
+      <c r="I20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" t="s">
+        <v>64</v>
+      </c>
+      <c r="L20" t="s">
+        <v>65</v>
+      </c>
+      <c r="M20" t="s">
+        <v>66</v>
+      </c>
+      <c r="N20">
+        <v>27</v>
+      </c>
+      <c r="O20">
+        <v>1.5</v>
+      </c>
+      <c r="P20">
+        <v>0.6</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>68</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0.6</v>
+      </c>
+      <c r="T20" t="s">
+        <v>70</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:52">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21">
+        <v>445</v>
+      </c>
+      <c r="I21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K21" t="s">
+        <v>64</v>
+      </c>
+      <c r="L21" t="s">
+        <v>65</v>
+      </c>
+      <c r="M21" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21">
+        <v>27</v>
+      </c>
+      <c r="O21">
+        <v>1.5</v>
+      </c>
+      <c r="P21">
+        <v>0.6</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>68</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0.6</v>
+      </c>
+      <c r="T21" t="s">
+        <v>70</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:52">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22">
+        <v>446</v>
+      </c>
+      <c r="I22" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" t="s">
+        <v>64</v>
+      </c>
+      <c r="K22" t="s">
+        <v>64</v>
+      </c>
+      <c r="L22" t="s">
+        <v>65</v>
+      </c>
+      <c r="M22" t="s">
+        <v>66</v>
+      </c>
+      <c r="N22">
+        <v>27</v>
+      </c>
+      <c r="O22">
+        <v>1.5</v>
+      </c>
+      <c r="P22">
+        <v>0.6</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>68</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0.6</v>
+      </c>
+      <c r="T22" t="s">
+        <v>70</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:52">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" t="s">
+        <v>59</v>
+      </c>
+      <c r="H23">
+        <v>447</v>
+      </c>
+      <c r="I23" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K23" t="s">
+        <v>64</v>
+      </c>
+      <c r="L23" t="s">
+        <v>65</v>
+      </c>
+      <c r="M23" t="s">
+        <v>66</v>
+      </c>
+      <c r="N23">
+        <v>27</v>
+      </c>
+      <c r="O23">
+        <v>1.5</v>
+      </c>
+      <c r="P23">
+        <v>0.6</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>68</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0.6</v>
+      </c>
+      <c r="T23" t="s">
+        <v>70</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:52">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24">
+        <v>448</v>
+      </c>
+      <c r="I24" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" t="s">
+        <v>64</v>
+      </c>
+      <c r="K24" t="s">
+        <v>64</v>
+      </c>
+      <c r="L24" t="s">
+        <v>65</v>
+      </c>
+      <c r="M24" t="s">
+        <v>66</v>
+      </c>
+      <c r="N24">
+        <v>27</v>
+      </c>
+      <c r="O24">
+        <v>1.5</v>
+      </c>
+      <c r="P24">
+        <v>0.6</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>68</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0.6</v>
+      </c>
+      <c r="T24" t="s">
+        <v>70</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>338.2035987392227</v>
+      </c>
+      <c r="W24">
+        <v>0.9895833333333334</v>
+      </c>
+      <c r="X24">
+        <v>235.8045877</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z24">
+        <v>338.2035987392227</v>
+      </c>
+      <c r="AA24">
+        <v>319.7926398351132</v>
+      </c>
+      <c r="AB24">
+        <v>18.41095890410959</v>
+      </c>
+      <c r="AC24">
+        <v>18.41095890410959</v>
+      </c>
+      <c r="AD24">
+        <v>448</v>
+      </c>
+      <c r="AE24">
+        <v>5.809518368950421</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AG24">
+        <v>0</v>
+      </c>
+      <c r="AH24">
+        <v>0.1640652466083759</v>
+      </c>
+      <c r="AI24">
+        <v>0.1640652466083759</v>
+      </c>
+      <c r="AJ24">
+        <v>0.1551339445046733</v>
+      </c>
+      <c r="AL24">
+        <v>81.8126350846957</v>
+      </c>
+      <c r="AM24">
+        <v>283.8478133040571</v>
+      </c>
+      <c r="AO24">
+        <v>34.35789473684211</v>
+      </c>
+      <c r="AP24">
+        <v>1850.755831578946</v>
+      </c>
+      <c r="AQ24">
+        <v>210.6411170784103</v>
+      </c>
+      <c r="AR24">
+        <v>2061.396948657356</v>
+      </c>
+      <c r="AS24">
+        <v>446.2578682383618</v>
+      </c>
+      <c r="AT24">
+        <v>1887.659128533829</v>
+      </c>
+      <c r="AU24">
+        <v>4.190691561245979</v>
+      </c>
+      <c r="AV24">
+        <v>284.3774156195714</v>
+      </c>
+      <c r="AW24">
+        <v>0.529602315514261</v>
+      </c>
+      <c r="AX24">
+        <v>136.3543918078262</v>
+      </c>
+      <c r="AY24">
+        <v>269.5435984532824</v>
+      </c>
+      <c r="AZ24">
+        <v>45.86780855363963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>